<commit_message>
Added Player Healing to server side attacks.
- This allows players to heal, ressurect and attempt to use life
  stealing affixes.

- Fixed Trinketry and the drop down list. Need to test that the crafying
  and trinkets actually get applied.

- Added Help Links.
</commit_message>
<xml_diff>
--- a/resources/data-imports/items/trinkets.xlsx
+++ b/resources/data-imports/items/trinkets.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Documents/flare/resources/data-imports/items/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE35095-E9B9-2744-96D7-52C1174272FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" r:id="rId4"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="135">
   <si>
     <t>id</t>
   </si>
@@ -221,12 +238,6 @@
     <t>Made of roots that bloom, this club sure is unique.</t>
   </si>
   <si>
-    <t>stave</t>
-  </si>
-  <si>
-    <t>weapon</t>
-  </si>
-  <si>
     <t>Corrupted Silk Headband of Hope</t>
   </si>
   <si>
@@ -423,19 +434,20 @@
   </si>
   <si>
     <t>Dance with the daggers, dance through the fear!</t>
+  </si>
+  <si>
+    <t>trinketry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -450,21 +462,35 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -754,86 +780,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="201" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="27" max="27" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="28" max="28" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="35" max="35" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="36" max="36" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="37" max="37" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="38" max="38" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="39" max="39" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="40" max="40" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="41" max="41" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="42" max="42" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="43" max="43" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="44" max="44" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="45" max="45" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="46" max="46" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="47" max="47" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="48" max="48" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="49" max="49" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="50" max="50" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="51" max="51" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="52" max="52" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="53" max="53" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="54" max="54" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="55" max="55" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="56" max="56" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="57" max="57" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="58" max="58" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="59" max="59" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="60" max="60" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="61" max="61" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="62" max="62" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="63" max="63" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="64" max="64" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="65" max="65" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="201" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="28" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="38" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="21" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="26" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1048,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>312105</v>
       </c>
@@ -1046,56 +1064,68 @@
       <c r="E2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2">
-        <v>280</v>
-      </c>
       <c r="J2">
-        <v>7000</v>
-      </c>
-      <c r="Q2">
-        <v>0.29</v>
-      </c>
-      <c r="S2">
-        <v>0.29</v>
-      </c>
-      <c r="U2">
-        <v>0.38</v>
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1E-3</v>
       </c>
       <c r="Y2">
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="AB2">
         <v>100</v>
       </c>
       <c r="AC2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF2">
-        <v>0.336</v>
+        <v>134</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
       </c>
       <c r="BI2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BJ2">
-        <v>0.1458</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="BK2">
-        <v>0.1458</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="BL2">
-        <v>0.1458</v>
+        <v>0.14580000000000001</v>
       </c>
       <c r="BM2">
-        <v>0.1458</v>
+        <v>0.14580000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:65">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>312123</v>
       </c>
@@ -1103,64 +1133,76 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3">
-        <v>730</v>
+        <v>69</v>
       </c>
       <c r="J3">
-        <v>250000000</v>
-      </c>
-      <c r="Q3">
-        <v>0.8</v>
-      </c>
-      <c r="S3">
-        <v>0.8</v>
-      </c>
-      <c r="U3">
-        <v>0.0908</v>
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1.6121212121212099E-2</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1.6121212121212099E-2</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1.6121212121212099E-2</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1.6121212121212099E-2</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1.6121212121212099E-2</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1.6121212121212099E-2</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1.6121212121212099E-2</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="AA3">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="AB3">
         <v>210</v>
       </c>
       <c r="AC3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF3">
-        <v>0.336</v>
+        <v>134</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
       </c>
       <c r="BI3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BJ3">
-        <v>0.4353</v>
+        <v>0.43530000000000002</v>
       </c>
       <c r="BK3">
-        <v>0.4353</v>
+        <v>0.43530000000000002</v>
       </c>
       <c r="BL3">
-        <v>0.4353</v>
+        <v>0.43530000000000002</v>
       </c>
       <c r="BM3">
-        <v>0.4353</v>
+        <v>0.43530000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>312124</v>
       </c>
@@ -1168,55 +1210,76 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4">
-        <v>740</v>
+        <v>71</v>
       </c>
       <c r="J4">
-        <v>500000000</v>
-      </c>
-      <c r="Q4">
-        <v>0.83</v>
-      </c>
-      <c r="S4">
-        <v>0.83</v>
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>15</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3.12424242424242E-2</v>
+      </c>
+      <c r="R4" s="1">
+        <v>3.12424242424242E-2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>3.12424242424242E-2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>3.12424242424242E-2</v>
+      </c>
+      <c r="U4" s="1">
+        <v>3.12424242424242E-2</v>
+      </c>
+      <c r="V4" s="1">
+        <v>3.12424242424242E-2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>3.12424242424242E-2</v>
       </c>
       <c r="Y4">
         <v>1</v>
       </c>
       <c r="AA4">
-        <v>210</v>
+        <v>20</v>
       </c>
       <c r="AB4">
         <v>220</v>
       </c>
       <c r="AC4" t="s">
-        <v>69</v>
+        <v>134</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
       </c>
       <c r="BI4">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BJ4">
-        <v>0.4514</v>
+        <v>0.45140000000000002</v>
       </c>
       <c r="BK4">
-        <v>0.4514</v>
+        <v>0.45140000000000002</v>
       </c>
       <c r="BL4">
-        <v>0.4514</v>
+        <v>0.45140000000000002</v>
       </c>
       <c r="BM4">
-        <v>0.4514</v>
+        <v>0.45140000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:65">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>312125</v>
       </c>
@@ -1224,55 +1287,76 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5">
-        <v>800</v>
+        <v>73</v>
       </c>
       <c r="J5">
-        <v>1000000000</v>
-      </c>
-      <c r="Q5">
-        <v>0.86</v>
-      </c>
-      <c r="S5">
-        <v>0.86</v>
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>4.6363636363636301E-2</v>
+      </c>
+      <c r="R5" s="1">
+        <v>4.6363636363636301E-2</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4.6363636363636301E-2</v>
+      </c>
+      <c r="T5" s="1">
+        <v>4.6363636363636301E-2</v>
+      </c>
+      <c r="U5" s="1">
+        <v>4.6363636363636301E-2</v>
+      </c>
+      <c r="V5" s="1">
+        <v>4.6363636363636301E-2</v>
+      </c>
+      <c r="W5" s="1">
+        <v>4.6363636363636301E-2</v>
       </c>
       <c r="Y5">
         <v>1</v>
       </c>
       <c r="AA5">
-        <v>215</v>
+        <v>30</v>
       </c>
       <c r="AB5">
         <v>220</v>
       </c>
       <c r="AC5" t="s">
-        <v>69</v>
+        <v>134</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
       </c>
       <c r="BI5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BJ5">
-        <v>0.4675</v>
+        <v>0.46750000000000003</v>
       </c>
       <c r="BK5">
-        <v>0.4675</v>
+        <v>0.46750000000000003</v>
       </c>
       <c r="BL5">
-        <v>0.4675</v>
+        <v>0.46750000000000003</v>
       </c>
       <c r="BM5">
-        <v>0.4675</v>
+        <v>0.46750000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:65">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>312126</v>
       </c>
@@ -1280,55 +1364,76 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6">
-        <v>845</v>
+        <v>75</v>
       </c>
       <c r="J6">
-        <v>2000000000</v>
-      </c>
-      <c r="Q6">
-        <v>0.9</v>
-      </c>
-      <c r="S6">
-        <v>0.9</v>
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>6.1484848484848399E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>6.1484848484848399E-2</v>
+      </c>
+      <c r="S6" s="1">
+        <v>6.1484848484848399E-2</v>
+      </c>
+      <c r="T6" s="1">
+        <v>6.1484848484848399E-2</v>
+      </c>
+      <c r="U6" s="1">
+        <v>6.1484848484848399E-2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>6.1484848484848399E-2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>6.1484848484848399E-2</v>
       </c>
       <c r="Y6">
         <v>1</v>
       </c>
       <c r="AA6">
-        <v>220</v>
+        <v>40</v>
       </c>
       <c r="AB6">
         <v>225</v>
       </c>
       <c r="AC6" t="s">
-        <v>69</v>
+        <v>134</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
       </c>
       <c r="BI6">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BJ6">
-        <v>0.4835</v>
+        <v>0.48349999999999999</v>
       </c>
       <c r="BK6">
-        <v>0.4835</v>
+        <v>0.48349999999999999</v>
       </c>
       <c r="BL6">
-        <v>0.4835</v>
+        <v>0.48349999999999999</v>
       </c>
       <c r="BM6">
-        <v>0.4835</v>
+        <v>0.48349999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:65">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>312127</v>
       </c>
@@ -1336,58 +1441,76 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D7" t="s">
         <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7">
-        <v>900</v>
+        <v>77</v>
       </c>
       <c r="J7">
-        <v>2100000000</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>70</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>7.6606060606060497E-2</v>
+      </c>
+      <c r="R7" s="1">
+        <v>7.6606060606060497E-2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>7.6606060606060497E-2</v>
+      </c>
+      <c r="T7" s="1">
+        <v>7.6606060606060497E-2</v>
+      </c>
+      <c r="U7" s="1">
+        <v>7.6606060606060497E-2</v>
+      </c>
+      <c r="V7" s="1">
+        <v>7.6606060606060497E-2</v>
+      </c>
+      <c r="W7" s="1">
+        <v>7.6606060606060497E-2</v>
       </c>
       <c r="Y7">
         <v>1</v>
       </c>
       <c r="AA7">
-        <v>225</v>
+        <v>50</v>
       </c>
       <c r="AB7">
         <v>228</v>
       </c>
       <c r="AC7" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL7">
         <v>1</v>
       </c>
       <c r="BI7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="BJ7">
-        <v>0.4996</v>
+        <v>0.49959999999999999</v>
       </c>
       <c r="BK7">
-        <v>0.4996</v>
+        <v>0.49959999999999999</v>
       </c>
       <c r="BL7">
-        <v>0.4996</v>
+        <v>0.49959999999999999</v>
       </c>
       <c r="BM7">
-        <v>0.4996</v>
+        <v>0.49959999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:65">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>312128</v>
       </c>
@@ -1395,58 +1518,76 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
         <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8">
-        <v>950</v>
+        <v>79</v>
       </c>
       <c r="J8">
-        <v>2200000000</v>
-      </c>
-      <c r="Q8">
-        <v>1.05</v>
-      </c>
-      <c r="S8">
-        <v>1.05</v>
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>90</v>
+      </c>
+      <c r="M8">
+        <v>110</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>9.1727272727272602E-2</v>
+      </c>
+      <c r="R8" s="1">
+        <v>9.1727272727272602E-2</v>
+      </c>
+      <c r="S8" s="1">
+        <v>9.1727272727272602E-2</v>
+      </c>
+      <c r="T8" s="1">
+        <v>9.1727272727272602E-2</v>
+      </c>
+      <c r="U8" s="1">
+        <v>9.1727272727272602E-2</v>
+      </c>
+      <c r="V8" s="1">
+        <v>9.1727272727272602E-2</v>
+      </c>
+      <c r="W8" s="1">
+        <v>9.1727272727272602E-2</v>
       </c>
       <c r="Y8">
         <v>1</v>
       </c>
       <c r="AA8">
-        <v>228</v>
+        <v>70</v>
       </c>
       <c r="AB8">
         <v>232</v>
       </c>
       <c r="AC8" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL8">
         <v>1</v>
       </c>
       <c r="BI8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="BJ8">
-        <v>0.5157</v>
+        <v>0.51570000000000005</v>
       </c>
       <c r="BK8">
-        <v>0.5157</v>
+        <v>0.51570000000000005</v>
       </c>
       <c r="BL8">
-        <v>0.5157</v>
+        <v>0.51570000000000005</v>
       </c>
       <c r="BM8">
-        <v>0.5157</v>
+        <v>0.51570000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:65">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>312129</v>
       </c>
@@ -1454,58 +1595,76 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9">
-        <v>1000</v>
+        <v>81</v>
       </c>
       <c r="J9">
-        <v>2300000000</v>
-      </c>
-      <c r="Q9">
-        <v>1.1</v>
-      </c>
-      <c r="S9">
-        <v>1.1</v>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>100</v>
+      </c>
+      <c r="M9">
+        <v>125</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.10684848484848469</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0.10684848484848469</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0.10684848484848469</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0.10684848484848469</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.10684848484848469</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.10684848484848469</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.10684848484848469</v>
       </c>
       <c r="Y9">
         <v>1</v>
       </c>
       <c r="AA9">
-        <v>232</v>
+        <v>90</v>
       </c>
       <c r="AB9">
         <v>250</v>
       </c>
       <c r="AC9" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL9">
         <v>1</v>
       </c>
       <c r="BI9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="BJ9">
-        <v>0.5318</v>
+        <v>0.53180000000000005</v>
       </c>
       <c r="BK9">
-        <v>0.5318</v>
+        <v>0.53180000000000005</v>
       </c>
       <c r="BL9">
-        <v>0.5318</v>
+        <v>0.53180000000000005</v>
       </c>
       <c r="BM9">
-        <v>0.5318</v>
+        <v>0.53180000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:65">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>312130</v>
       </c>
@@ -1513,58 +1672,76 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10">
-        <v>1100</v>
+        <v>83</v>
       </c>
       <c r="J10">
-        <v>2400000000</v>
-      </c>
-      <c r="Q10">
-        <v>1.15</v>
-      </c>
-      <c r="S10">
-        <v>1.15</v>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>150</v>
+      </c>
+      <c r="M10">
+        <v>175</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.1219696969696968</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.1219696969696968</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0.1219696969696968</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0.1219696969696968</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0.1219696969696968</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.1219696969696968</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.1219696969696968</v>
       </c>
       <c r="Y10">
         <v>1</v>
       </c>
       <c r="AA10">
-        <v>235</v>
+        <v>110</v>
       </c>
       <c r="AB10">
         <v>250</v>
       </c>
       <c r="AC10" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL10">
         <v>1</v>
       </c>
       <c r="BI10">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="BJ10">
-        <v>0.5479</v>
+        <v>0.54790000000000005</v>
       </c>
       <c r="BK10">
-        <v>0.5479</v>
+        <v>0.54790000000000005</v>
       </c>
       <c r="BL10">
-        <v>0.5479</v>
+        <v>0.54790000000000005</v>
       </c>
       <c r="BM10">
-        <v>0.5479</v>
+        <v>0.54790000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:65">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>312131</v>
       </c>
@@ -1572,58 +1749,76 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
         <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11">
-        <v>1200</v>
+        <v>85</v>
       </c>
       <c r="J11">
-        <v>2800000000</v>
-      </c>
-      <c r="Q11">
-        <v>1.2</v>
-      </c>
-      <c r="S11">
-        <v>1.2</v>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>300</v>
+      </c>
+      <c r="M11">
+        <v>180</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.1370909090909089</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0.1370909090909089</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0.1370909090909089</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0.1370909090909089</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0.1370909090909089</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.1370909090909089</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0.1370909090909089</v>
       </c>
       <c r="Y11">
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="AB11">
         <v>270</v>
       </c>
       <c r="AC11" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL11">
         <v>1</v>
       </c>
       <c r="BI11">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BJ11">
-        <v>0.564</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="BK11">
-        <v>0.564</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="BL11">
-        <v>0.564</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="BM11">
-        <v>0.564</v>
+        <v>0.56399999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:65">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>312132</v>
       </c>
@@ -1631,58 +1826,76 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12">
-        <v>1300</v>
+        <v>87</v>
       </c>
       <c r="J12">
-        <v>3200000000</v>
-      </c>
-      <c r="Q12">
-        <v>1.35</v>
-      </c>
-      <c r="S12">
-        <v>1.35</v>
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>600</v>
+      </c>
+      <c r="M12">
+        <v>200</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.15221212121212099</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0.15221212121212099</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0.15221212121212099</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0.15221212121212099</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0.15221212121212099</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.15221212121212099</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.15221212121212099</v>
       </c>
       <c r="Y12">
         <v>1</v>
       </c>
       <c r="AA12">
-        <v>245</v>
+        <v>130</v>
       </c>
       <c r="AB12">
         <v>270</v>
       </c>
       <c r="AC12" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL12">
         <v>1</v>
       </c>
       <c r="BI12">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BJ12">
-        <v>0.5801</v>
+        <v>0.58009999999999995</v>
       </c>
       <c r="BK12">
-        <v>0.5801</v>
+        <v>0.58009999999999995</v>
       </c>
       <c r="BL12">
-        <v>0.5801</v>
+        <v>0.58009999999999995</v>
       </c>
       <c r="BM12">
-        <v>0.5801</v>
+        <v>0.58009999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:65">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>312133</v>
       </c>
@@ -1690,58 +1903,76 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
         <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13">
-        <v>1400</v>
+        <v>89</v>
       </c>
       <c r="J13">
-        <v>3300000000</v>
-      </c>
-      <c r="Q13">
-        <v>1.4</v>
-      </c>
-      <c r="S13">
-        <v>1.4</v>
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>700</v>
+      </c>
+      <c r="M13">
+        <v>250</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.16733333333333308</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.16733333333333308</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0.16733333333333308</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0.16733333333333308</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0.16733333333333308</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.16733333333333308</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0.16733333333333308</v>
       </c>
       <c r="Y13">
         <v>1</v>
       </c>
       <c r="AA13">
-        <v>253</v>
+        <v>140</v>
       </c>
       <c r="AB13">
         <v>270</v>
       </c>
       <c r="AC13" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL13">
         <v>1</v>
       </c>
       <c r="BI13">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BJ13">
-        <v>0.5961</v>
+        <v>0.59609999999999996</v>
       </c>
       <c r="BK13">
-        <v>0.5961</v>
+        <v>0.59609999999999996</v>
       </c>
       <c r="BL13">
-        <v>0.5961</v>
+        <v>0.59609999999999996</v>
       </c>
       <c r="BM13">
-        <v>0.5961</v>
+        <v>0.59609999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:65">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>312134</v>
       </c>
@@ -1749,58 +1980,76 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
         <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14">
-        <v>1500</v>
+        <v>91</v>
       </c>
       <c r="J14">
-        <v>3500000000</v>
-      </c>
-      <c r="Q14">
-        <v>1.43</v>
-      </c>
-      <c r="S14">
-        <v>1.43</v>
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M14">
+        <v>500</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0.1824545454545452</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0.1824545454545452</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0.1824545454545452</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0.1824545454545452</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.1824545454545452</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.1824545454545452</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0.1824545454545452</v>
       </c>
       <c r="Y14">
         <v>1</v>
       </c>
       <c r="AA14">
-        <v>260</v>
+        <v>150</v>
       </c>
       <c r="AB14">
         <v>270</v>
       </c>
       <c r="AC14" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL14">
         <v>1</v>
       </c>
       <c r="BI14">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BJ14">
-        <v>0.6122</v>
+        <v>0.61219999999999997</v>
       </c>
       <c r="BK14">
-        <v>0.6122</v>
+        <v>0.61219999999999997</v>
       </c>
       <c r="BL14">
-        <v>0.6122</v>
+        <v>0.61219999999999997</v>
       </c>
       <c r="BM14">
-        <v>0.6122</v>
+        <v>0.61219999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>312135</v>
       </c>
@@ -1808,58 +2057,76 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
         <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15">
-        <v>1600</v>
+        <v>93</v>
       </c>
       <c r="J15">
-        <v>3700000000</v>
-      </c>
-      <c r="Q15">
-        <v>1.47</v>
-      </c>
-      <c r="S15">
-        <v>1.47</v>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1500</v>
+      </c>
+      <c r="M15">
+        <v>550</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0.19757575757575729</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0.19757575757575729</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.19757575757575729</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.19757575757575729</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0.19757575757575729</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.19757575757575729</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0.19757575757575729</v>
       </c>
       <c r="Y15">
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>265</v>
+        <v>160</v>
       </c>
       <c r="AB15">
         <v>280</v>
       </c>
       <c r="AC15" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL15">
         <v>1</v>
       </c>
       <c r="BI15">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BJ15">
-        <v>0.6283</v>
+        <v>0.62829999999999997</v>
       </c>
       <c r="BK15">
-        <v>0.6283</v>
+        <v>0.62829999999999997</v>
       </c>
       <c r="BL15">
-        <v>0.6283</v>
+        <v>0.62829999999999997</v>
       </c>
       <c r="BM15">
-        <v>0.6283</v>
+        <v>0.62829999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>312136</v>
       </c>
@@ -1867,58 +2134,76 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
         <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16">
-        <v>1700</v>
+        <v>95</v>
       </c>
       <c r="J16">
-        <v>4200000000</v>
-      </c>
-      <c r="Q16">
-        <v>1.5</v>
-      </c>
-      <c r="S16">
-        <v>1.5</v>
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1800</v>
+      </c>
+      <c r="M16">
+        <v>700</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.21269696969696938</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.21269696969696938</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.21269696969696938</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.21269696969696938</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.21269696969696938</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.21269696969696938</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0.21269696969696938</v>
       </c>
       <c r="Y16">
         <v>1</v>
       </c>
       <c r="AA16">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="AB16">
         <v>290</v>
       </c>
       <c r="AC16" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL16">
         <v>1</v>
       </c>
       <c r="BI16">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="BJ16">
-        <v>0.6444</v>
+        <v>0.64439999999999997</v>
       </c>
       <c r="BK16">
-        <v>0.6444</v>
+        <v>0.64439999999999997</v>
       </c>
       <c r="BL16">
-        <v>0.6444</v>
+        <v>0.64439999999999997</v>
       </c>
       <c r="BM16">
-        <v>0.6444</v>
+        <v>0.64439999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:65">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>312137</v>
       </c>
@@ -1926,58 +2211,76 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
         <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
-      </c>
-      <c r="G17">
-        <v>1800</v>
+        <v>97</v>
       </c>
       <c r="J17">
-        <v>4400000000</v>
-      </c>
-      <c r="Q17">
-        <v>1.55</v>
-      </c>
-      <c r="S17">
-        <v>1.55</v>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M17">
+        <v>875</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.2278181818181815</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0.2278181818181815</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.2278181818181815</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0.2278181818181815</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.2278181818181815</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.2278181818181815</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0.2278181818181815</v>
       </c>
       <c r="Y17">
         <v>1</v>
       </c>
       <c r="AA17">
-        <v>275</v>
+        <v>180</v>
       </c>
       <c r="AB17">
         <v>300</v>
       </c>
       <c r="AC17" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL17">
         <v>1</v>
       </c>
       <c r="BI17">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="BJ17">
-        <v>0.6605</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="BK17">
-        <v>0.6605</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="BL17">
-        <v>0.6605</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="BM17">
-        <v>0.6605</v>
+        <v>0.66049999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:65">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>312138</v>
       </c>
@@ -1985,58 +2288,76 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18">
-        <v>1900</v>
+        <v>99</v>
       </c>
       <c r="J18">
-        <v>4600000000</v>
-      </c>
-      <c r="Q18">
-        <v>1.63</v>
-      </c>
-      <c r="S18">
-        <v>1.63</v>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3000</v>
+      </c>
+      <c r="M18">
+        <v>900</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0.24293939393939359</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0.24293939393939359</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0.24293939393939359</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0.24293939393939359</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0.24293939393939359</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0.24293939393939359</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0.24293939393939359</v>
       </c>
       <c r="Y18">
         <v>1</v>
       </c>
       <c r="AA18">
-        <v>280</v>
+        <v>190</v>
       </c>
       <c r="AB18">
         <v>310</v>
       </c>
       <c r="AC18" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL18">
         <v>1</v>
       </c>
       <c r="BI18">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="BJ18">
-        <v>0.6766</v>
+        <v>0.67659999999999998</v>
       </c>
       <c r="BK18">
-        <v>0.6766</v>
+        <v>0.67659999999999998</v>
       </c>
       <c r="BL18">
-        <v>0.6766</v>
+        <v>0.67659999999999998</v>
       </c>
       <c r="BM18">
-        <v>0.6766</v>
+        <v>0.67659999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:65">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>312139</v>
       </c>
@@ -2044,58 +2365,76 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
         <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19">
-        <v>2000</v>
+        <v>101</v>
       </c>
       <c r="J19">
-        <v>5000000000</v>
-      </c>
-      <c r="Q19">
-        <v>1.68</v>
-      </c>
-      <c r="S19">
-        <v>1.68</v>
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>3500</v>
+      </c>
+      <c r="M19">
+        <v>950</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.25806060606060571</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0.25806060606060571</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0.25806060606060571</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0.25806060606060571</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0.25806060606060571</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0.25806060606060571</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0.25806060606060571</v>
       </c>
       <c r="Y19">
         <v>1</v>
       </c>
       <c r="AA19">
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="AB19">
         <v>320</v>
       </c>
       <c r="AC19" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL19">
         <v>1</v>
       </c>
       <c r="BI19">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="BJ19">
-        <v>0.6926</v>
+        <v>0.69259999999999999</v>
       </c>
       <c r="BK19">
-        <v>0.6926</v>
+        <v>0.69259999999999999</v>
       </c>
       <c r="BL19">
-        <v>0.6926</v>
+        <v>0.69259999999999999</v>
       </c>
       <c r="BM19">
-        <v>0.6926</v>
+        <v>0.69259999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:65">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>312140</v>
       </c>
@@ -2103,43 +2442,61 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
         <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20">
-        <v>2100</v>
+        <v>103</v>
       </c>
       <c r="J20">
-        <v>5300000000</v>
-      </c>
-      <c r="Q20">
-        <v>1.73</v>
-      </c>
-      <c r="S20">
-        <v>1.73</v>
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>4000</v>
+      </c>
+      <c r="M20">
+        <v>975</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.2731818181818178</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0.2731818181818178</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0.2731818181818178</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0.2731818181818178</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0.2731818181818178</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.2731818181818178</v>
+      </c>
+      <c r="W20" s="1">
+        <v>0.2731818181818178</v>
       </c>
       <c r="Y20">
         <v>1</v>
       </c>
       <c r="AA20">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="AB20">
         <v>320</v>
       </c>
       <c r="AC20" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL20">
         <v>1</v>
       </c>
       <c r="BI20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="BJ20">
         <v>0.7087</v>
@@ -2154,7 +2511,7 @@
         <v>0.7087</v>
       </c>
     </row>
-    <row r="21" spans="1:65">
+    <row r="21" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>312141</v>
       </c>
@@ -2162,43 +2519,61 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
         <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21">
-        <v>2200</v>
+        <v>105</v>
       </c>
       <c r="J21">
-        <v>5600000000</v>
-      </c>
-      <c r="Q21">
-        <v>1.76</v>
-      </c>
-      <c r="S21">
-        <v>1.76</v>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>5000</v>
+      </c>
+      <c r="M21">
+        <v>1000</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0.28830303030302989</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0.28830303030302989</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0.28830303030302989</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0.28830303030302989</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0.28830303030302989</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0.28830303030302989</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0.28830303030302989</v>
       </c>
       <c r="Y21">
         <v>1</v>
       </c>
       <c r="AA21">
-        <v>310</v>
+        <v>240</v>
       </c>
       <c r="AB21">
         <v>330</v>
       </c>
       <c r="AC21" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL21">
         <v>1</v>
       </c>
       <c r="BI21">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="BJ21">
         <v>0.7248</v>
@@ -2213,7 +2588,7 @@
         <v>0.7248</v>
       </c>
     </row>
-    <row r="22" spans="1:65">
+    <row r="22" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>312142</v>
       </c>
@@ -2221,43 +2596,61 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
         <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22">
-        <v>2300</v>
+        <v>107</v>
       </c>
       <c r="J22">
-        <v>5800000000</v>
-      </c>
-      <c r="Q22">
-        <v>1.8</v>
-      </c>
-      <c r="S22">
-        <v>1.8</v>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5500</v>
+      </c>
+      <c r="M22">
+        <v>1100</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0.30342424242424199</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0.30342424242424199</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0.30342424242424199</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0.30342424242424199</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0.30342424242424199</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0.30342424242424199</v>
+      </c>
+      <c r="W22" s="1">
+        <v>0.30342424242424199</v>
       </c>
       <c r="Y22">
         <v>1</v>
       </c>
       <c r="AA22">
-        <v>318</v>
+        <v>260</v>
       </c>
       <c r="AB22">
         <v>340</v>
       </c>
       <c r="AC22" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL22">
         <v>1</v>
       </c>
       <c r="BI22">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="BJ22">
         <v>0.7409</v>
@@ -2272,7 +2665,7 @@
         <v>0.7409</v>
       </c>
     </row>
-    <row r="23" spans="1:65">
+    <row r="23" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>312143</v>
       </c>
@@ -2280,58 +2673,76 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
         <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23">
-        <v>2400</v>
+        <v>109</v>
       </c>
       <c r="J23">
-        <v>6000000000</v>
-      </c>
-      <c r="Q23">
-        <v>1.87</v>
-      </c>
-      <c r="S23">
-        <v>1.87</v>
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>6000</v>
+      </c>
+      <c r="M23">
+        <v>1150</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0.31854545454545408</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0.31854545454545408</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0.31854545454545408</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0.31854545454545408</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0.31854545454545408</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0.31854545454545408</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0.31854545454545408</v>
       </c>
       <c r="Y23">
         <v>1</v>
       </c>
       <c r="AA23">
-        <v>324</v>
+        <v>280</v>
       </c>
       <c r="AB23">
         <v>350</v>
       </c>
       <c r="AC23" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL23">
         <v>1</v>
       </c>
       <c r="BI23">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BJ23">
-        <v>0.757</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="BK23">
-        <v>0.757</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="BL23">
-        <v>0.757</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="BM23">
-        <v>0.757</v>
+        <v>0.75700000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:65">
+    <row r="24" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>312144</v>
       </c>
@@ -2339,58 +2750,76 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
         <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24">
-        <v>2600</v>
+        <v>111</v>
       </c>
       <c r="J24">
-        <v>10000000000</v>
-      </c>
-      <c r="Q24">
-        <v>2.08</v>
-      </c>
-      <c r="S24">
-        <v>2.08</v>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>7000</v>
+      </c>
+      <c r="M24">
+        <v>1200</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0.33366666666666617</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0.33366666666666617</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0.33366666666666617</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0.33366666666666617</v>
+      </c>
+      <c r="U24" s="1">
+        <v>0.33366666666666617</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0.33366666666666617</v>
+      </c>
+      <c r="W24" s="1">
+        <v>0.33366666666666617</v>
       </c>
       <c r="Y24">
         <v>1</v>
       </c>
       <c r="AA24">
-        <v>340</v>
+        <v>300</v>
       </c>
       <c r="AB24">
         <v>370</v>
       </c>
       <c r="AC24" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL24">
         <v>1</v>
       </c>
       <c r="BI24">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ24">
-        <v>0.7731</v>
+        <v>0.77310000000000001</v>
       </c>
       <c r="BK24">
-        <v>0.7731</v>
+        <v>0.77310000000000001</v>
       </c>
       <c r="BL24">
-        <v>0.7731</v>
+        <v>0.77310000000000001</v>
       </c>
       <c r="BM24">
-        <v>0.7731</v>
+        <v>0.77310000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:65">
+    <row r="25" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>312145</v>
       </c>
@@ -2398,58 +2827,76 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
         <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25">
-        <v>2700</v>
+        <v>113</v>
       </c>
       <c r="J25">
-        <v>12000000000</v>
-      </c>
-      <c r="Q25">
-        <v>2.12</v>
-      </c>
-      <c r="S25">
-        <v>2.12</v>
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>8000</v>
+      </c>
+      <c r="M25">
+        <v>1250</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0.34878787878787831</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0.34878787878787831</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0.34878787878787831</v>
+      </c>
+      <c r="T25" s="1">
+        <v>0.34878787878787831</v>
+      </c>
+      <c r="U25" s="1">
+        <v>0.34878787878787831</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0.34878787878787831</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0.34878787878787831</v>
       </c>
       <c r="Y25">
         <v>1</v>
       </c>
       <c r="AA25">
-        <v>350</v>
+        <v>320</v>
       </c>
       <c r="AB25">
         <v>380</v>
       </c>
       <c r="AC25" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL25">
         <v>1</v>
       </c>
       <c r="BI25">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ25">
-        <v>0.7892</v>
+        <v>0.78920000000000001</v>
       </c>
       <c r="BK25">
-        <v>0.7892</v>
+        <v>0.78920000000000001</v>
       </c>
       <c r="BL25">
-        <v>0.7892</v>
+        <v>0.78920000000000001</v>
       </c>
       <c r="BM25">
-        <v>0.7892</v>
+        <v>0.78920000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:65">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>312146</v>
       </c>
@@ -2457,58 +2904,76 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
         <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>117</v>
-      </c>
-      <c r="G26">
-        <v>2800</v>
+        <v>115</v>
       </c>
       <c r="J26">
-        <v>16000000000</v>
-      </c>
-      <c r="Q26">
-        <v>2.16</v>
-      </c>
-      <c r="S26">
-        <v>2.16</v>
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>9000</v>
+      </c>
+      <c r="M26">
+        <v>1500</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>0.3639090909090904</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0.3639090909090904</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0.3639090909090904</v>
+      </c>
+      <c r="T26" s="1">
+        <v>0.3639090909090904</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0.3639090909090904</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0.3639090909090904</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0.3639090909090904</v>
       </c>
       <c r="Y26">
         <v>1</v>
       </c>
       <c r="AA26">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="AB26">
         <v>380</v>
       </c>
       <c r="AC26" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL26">
         <v>1</v>
       </c>
       <c r="BI26">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ26">
-        <v>0.8052</v>
+        <v>0.80520000000000003</v>
       </c>
       <c r="BK26">
-        <v>0.8052</v>
+        <v>0.80520000000000003</v>
       </c>
       <c r="BL26">
-        <v>0.8052</v>
+        <v>0.80520000000000003</v>
       </c>
       <c r="BM26">
-        <v>0.8052</v>
+        <v>0.80520000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:65">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>312147</v>
       </c>
@@ -2516,58 +2981,76 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
         <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>119</v>
-      </c>
-      <c r="G27">
-        <v>2900</v>
+        <v>117</v>
       </c>
       <c r="J27">
-        <v>18000000000</v>
-      </c>
-      <c r="Q27">
-        <v>2.18</v>
-      </c>
-      <c r="S27">
-        <v>2.18</v>
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>9500</v>
+      </c>
+      <c r="M27">
+        <v>1700</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>0.3790303030303025</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0.3790303030303025</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0.3790303030303025</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0.3790303030303025</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0.3790303030303025</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0.3790303030303025</v>
+      </c>
+      <c r="W27" s="1">
+        <v>0.3790303030303025</v>
       </c>
       <c r="Y27">
         <v>1</v>
       </c>
       <c r="AA27">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="AB27">
         <v>380</v>
       </c>
       <c r="AC27" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL27">
         <v>1</v>
       </c>
       <c r="BI27">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ27">
-        <v>0.8213</v>
+        <v>0.82130000000000003</v>
       </c>
       <c r="BK27">
-        <v>0.8213</v>
+        <v>0.82130000000000003</v>
       </c>
       <c r="BL27">
-        <v>0.8213</v>
+        <v>0.82130000000000003</v>
       </c>
       <c r="BM27">
-        <v>0.8213</v>
+        <v>0.82130000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:65">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>312148</v>
       </c>
@@ -2575,58 +3058,76 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
         <v>66</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
-      </c>
-      <c r="G28">
-        <v>3000</v>
+        <v>119</v>
       </c>
       <c r="J28">
-        <v>22000000000</v>
-      </c>
-      <c r="Q28">
-        <v>2.24</v>
-      </c>
-      <c r="S28">
-        <v>2.24</v>
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="M28">
+        <v>1800</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0.39415151515151459</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0.39415151515151459</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0.39415151515151459</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0.39415151515151459</v>
+      </c>
+      <c r="U28" s="1">
+        <v>0.39415151515151459</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0.39415151515151459</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0.39415151515151459</v>
       </c>
       <c r="Y28">
         <v>1</v>
       </c>
       <c r="AA28">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="AB28">
         <v>380</v>
       </c>
       <c r="AC28" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL28">
         <v>1</v>
       </c>
       <c r="BI28">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ28">
-        <v>0.8374</v>
+        <v>0.83740000000000003</v>
       </c>
       <c r="BK28">
-        <v>0.8374</v>
+        <v>0.83740000000000003</v>
       </c>
       <c r="BL28">
-        <v>0.8374</v>
+        <v>0.83740000000000003</v>
       </c>
       <c r="BM28">
-        <v>0.8374</v>
+        <v>0.83740000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:65">
+    <row r="29" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>312149</v>
       </c>
@@ -2634,58 +3135,76 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D29" t="s">
         <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>123</v>
-      </c>
-      <c r="G29">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="J29">
-        <v>24000000000</v>
-      </c>
-      <c r="Q29">
-        <v>2.26</v>
-      </c>
-      <c r="S29">
-        <v>2.26</v>
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>12000</v>
+      </c>
+      <c r="M29">
+        <v>1900</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0.40927272727272668</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0.40927272727272668</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0.40927272727272668</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0.40927272727272668</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0.40927272727272668</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0.40927272727272668</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0.40927272727272668</v>
       </c>
       <c r="Y29">
         <v>1</v>
       </c>
       <c r="AA29">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="AB29">
         <v>380</v>
       </c>
       <c r="AC29" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL29">
         <v>1</v>
       </c>
       <c r="BI29">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ29">
-        <v>0.8535</v>
+        <v>0.85350000000000004</v>
       </c>
       <c r="BK29">
-        <v>0.8535</v>
+        <v>0.85350000000000004</v>
       </c>
       <c r="BL29">
-        <v>0.8535</v>
+        <v>0.85350000000000004</v>
       </c>
       <c r="BM29">
-        <v>0.8535</v>
+        <v>0.85350000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:65">
+    <row r="30" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>312150</v>
       </c>
@@ -2693,58 +3212,76 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
         <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>125</v>
-      </c>
-      <c r="G30">
-        <v>3200</v>
+        <v>123</v>
       </c>
       <c r="J30">
-        <v>26000000000</v>
-      </c>
-      <c r="Q30">
-        <v>2.28</v>
-      </c>
-      <c r="S30">
-        <v>2.28</v>
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>15000</v>
+      </c>
+      <c r="M30">
+        <v>2000</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0.42439393939393877</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0.42439393939393877</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0.42439393939393877</v>
+      </c>
+      <c r="T30" s="1">
+        <v>0.42439393939393877</v>
+      </c>
+      <c r="U30" s="1">
+        <v>0.42439393939393877</v>
+      </c>
+      <c r="V30" s="1">
+        <v>0.42439393939393877</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0.42439393939393877</v>
       </c>
       <c r="Y30">
         <v>1</v>
       </c>
       <c r="AA30">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="AB30">
         <v>385</v>
       </c>
       <c r="AC30" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL30">
         <v>1</v>
       </c>
       <c r="BI30">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ30">
-        <v>0.8696</v>
+        <v>0.86960000000000004</v>
       </c>
       <c r="BK30">
-        <v>0.8696</v>
+        <v>0.86960000000000004</v>
       </c>
       <c r="BL30">
-        <v>0.8696</v>
+        <v>0.86960000000000004</v>
       </c>
       <c r="BM30">
-        <v>0.8696</v>
+        <v>0.86960000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:65">
+    <row r="31" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>312151</v>
       </c>
@@ -2752,25 +3289,43 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D31" t="s">
         <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
-      </c>
-      <c r="G31">
-        <v>3300</v>
+        <v>125</v>
       </c>
       <c r="J31">
-        <v>28000000000</v>
-      </c>
-      <c r="Q31">
-        <v>2.32</v>
-      </c>
-      <c r="S31">
-        <v>2.32</v>
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>18000</v>
+      </c>
+      <c r="M31">
+        <v>2200</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0.43951515151515091</v>
+      </c>
+      <c r="R31" s="1">
+        <v>0.43951515151515091</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0.43951515151515091</v>
+      </c>
+      <c r="T31" s="1">
+        <v>0.43951515151515091</v>
+      </c>
+      <c r="U31" s="1">
+        <v>0.43951515151515091</v>
+      </c>
+      <c r="V31" s="1">
+        <v>0.43951515151515091</v>
+      </c>
+      <c r="W31" s="1">
+        <v>0.43951515151515091</v>
       </c>
       <c r="Y31">
         <v>1</v>
@@ -2782,28 +3337,28 @@
         <v>385</v>
       </c>
       <c r="AC31" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL31">
         <v>1</v>
       </c>
       <c r="BI31">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="BJ31">
-        <v>0.8857</v>
+        <v>0.88570000000000004</v>
       </c>
       <c r="BK31">
-        <v>0.8857</v>
+        <v>0.88570000000000004</v>
       </c>
       <c r="BL31">
-        <v>0.8857</v>
+        <v>0.88570000000000004</v>
       </c>
       <c r="BM31">
-        <v>0.8857</v>
+        <v>0.88570000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:65">
+    <row r="32" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>312152</v>
       </c>
@@ -2811,58 +3366,76 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D32" t="s">
         <v>66</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
-      </c>
-      <c r="G32">
-        <v>3400</v>
+        <v>127</v>
       </c>
       <c r="J32">
-        <v>30000000000</v>
-      </c>
-      <c r="Q32">
-        <v>2.34</v>
-      </c>
-      <c r="S32">
-        <v>2.34</v>
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>20000</v>
+      </c>
+      <c r="M32">
+        <v>2500</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0.45463636363636301</v>
+      </c>
+      <c r="R32" s="1">
+        <v>0.45463636363636301</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0.45463636363636301</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0.45463636363636301</v>
+      </c>
+      <c r="U32" s="1">
+        <v>0.45463636363636301</v>
+      </c>
+      <c r="V32" s="1">
+        <v>0.45463636363636301</v>
+      </c>
+      <c r="W32" s="1">
+        <v>0.45463636363636301</v>
       </c>
       <c r="Y32">
         <v>1</v>
       </c>
       <c r="AA32">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="AB32">
         <v>390</v>
       </c>
       <c r="AC32" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL32">
         <v>1</v>
       </c>
       <c r="BI32">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BJ32">
-        <v>0.9017</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="BK32">
-        <v>0.9017</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="BL32">
-        <v>0.9017</v>
+        <v>0.90169999999999995</v>
       </c>
       <c r="BM32">
-        <v>0.9017</v>
+        <v>0.90169999999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:65">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>312153</v>
       </c>
@@ -2870,58 +3443,76 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
         <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
-      </c>
-      <c r="G33">
-        <v>3500</v>
+        <v>129</v>
       </c>
       <c r="J33">
-        <v>32000000000</v>
-      </c>
-      <c r="Q33">
-        <v>2.36</v>
-      </c>
-      <c r="S33">
-        <v>2.36</v>
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>30000</v>
+      </c>
+      <c r="M33">
+        <v>3000</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0.4697575757575751</v>
+      </c>
+      <c r="R33" s="1">
+        <v>0.4697575757575751</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0.4697575757575751</v>
+      </c>
+      <c r="T33" s="1">
+        <v>0.4697575757575751</v>
+      </c>
+      <c r="U33" s="1">
+        <v>0.4697575757575751</v>
+      </c>
+      <c r="V33" s="1">
+        <v>0.4697575757575751</v>
+      </c>
+      <c r="W33" s="1">
+        <v>0.4697575757575751</v>
       </c>
       <c r="Y33">
         <v>1</v>
       </c>
       <c r="AA33">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="AB33">
         <v>395</v>
       </c>
       <c r="AC33" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL33">
         <v>1</v>
       </c>
       <c r="BI33">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BJ33">
-        <v>0.9178</v>
+        <v>0.91779999999999995</v>
       </c>
       <c r="BK33">
-        <v>0.9178</v>
+        <v>0.91779999999999995</v>
       </c>
       <c r="BL33">
-        <v>0.9178</v>
+        <v>0.91779999999999995</v>
       </c>
       <c r="BM33">
-        <v>0.9178</v>
+        <v>0.91779999999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:65">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>312154</v>
       </c>
@@ -2929,58 +3520,76 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D34" t="s">
         <v>66</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
-      </c>
-      <c r="G34">
-        <v>3600</v>
+        <v>131</v>
       </c>
       <c r="J34">
-        <v>34000000000</v>
-      </c>
-      <c r="Q34">
-        <v>2.38</v>
-      </c>
-      <c r="S34">
-        <v>2.38</v>
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>40000</v>
+      </c>
+      <c r="M34">
+        <v>4000</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0.48487878787878719</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0.48487878787878719</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0.48487878787878719</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0.48487878787878719</v>
+      </c>
+      <c r="U34" s="1">
+        <v>0.48487878787878719</v>
+      </c>
+      <c r="V34" s="1">
+        <v>0.48487878787878719</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0.48487878787878719</v>
       </c>
       <c r="Y34">
         <v>1</v>
       </c>
       <c r="AA34">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="AB34">
         <v>399</v>
       </c>
       <c r="AC34" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL34">
         <v>1</v>
       </c>
       <c r="BI34">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BJ34">
-        <v>0.9339</v>
+        <v>0.93389999999999995</v>
       </c>
       <c r="BK34">
-        <v>0.9339</v>
+        <v>0.93389999999999995</v>
       </c>
       <c r="BL34">
-        <v>0.9339</v>
+        <v>0.93389999999999995</v>
       </c>
       <c r="BM34">
-        <v>0.9339</v>
+        <v>0.93389999999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:65">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>312155</v>
       </c>
@@ -2988,25 +3597,43 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D35" t="s">
         <v>66</v>
       </c>
       <c r="E35" t="s">
-        <v>135</v>
-      </c>
-      <c r="G35">
-        <v>3700</v>
+        <v>133</v>
       </c>
       <c r="J35">
-        <v>36000000000</v>
-      </c>
-      <c r="Q35">
-        <v>2.4</v>
-      </c>
-      <c r="S35">
-        <v>2.4</v>
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>50000</v>
+      </c>
+      <c r="M35">
+        <v>5000</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0.49999999999999928</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0.49999999999999928</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0.49999999999999928</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0.49999999999999928</v>
+      </c>
+      <c r="U35" s="1">
+        <v>0.49999999999999928</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0.49999999999999928</v>
+      </c>
+      <c r="W35" s="1">
+        <v>0.49999999999999928</v>
       </c>
       <c r="Y35">
         <v>1</v>
@@ -3018,13 +3645,13 @@
         <v>401</v>
       </c>
       <c r="AC35" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="AL35">
         <v>1</v>
       </c>
       <c r="BI35">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BJ35">
         <v>0.95</v>
@@ -3040,18 +3667,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>